<commit_message>
Add podman x86 benchmarks
</commit_message>
<xml_diff>
--- a/results/Global performance comparison.xlsx
+++ b/results/Global performance comparison.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a039662\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohan/containers-comparison/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF2E4477-F3AD-4318-BB91-C605C200C3CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433638A2-4688-C04E-A229-EEFF6895732B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{2794598E-EB7C-45E9-952E-510353A79499}"/>
+    <workbookView xWindow="-10540" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="6" xr2:uid="{2794598E-EB7C-45E9-952E-510353A79499}"/>
   </bookViews>
   <sheets>
     <sheet name="build" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="21">
   <si>
     <t>backend</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Docker X86</t>
   </si>
   <si>
-    <t>rkt X86</t>
-  </si>
-  <si>
     <t>LXC ARM</t>
   </si>
   <si>
@@ -102,16 +99,23 @@
   </si>
   <si>
     <t xml:space="preserve">MEMORY USAGE IDLE (en MiB) </t>
+  </si>
+  <si>
+    <t>podman X86</t>
+  </si>
+  <si>
+    <t>podman ARM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,6 +131,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,7 +154,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -185,24 +203,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,13 +570,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{141B6A51-865E-45EA-8B42-AEDBB16E509A}">
   <dimension ref="C5:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView zoomScale="206" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
         <v>3</v>
@@ -534,10 +585,13 @@
         <v>4</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
@@ -547,9 +601,14 @@
       <c r="E6" s="1">
         <v>17</v>
       </c>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F6" s="1">
+        <v>33</v>
+      </c>
+      <c r="G6" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C7" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,9 +618,14 @@
       <c r="E7" s="1">
         <v>15</v>
       </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="F7" s="1">
+        <v>48</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
         <v>1</v>
       </c>
@@ -571,25 +635,30 @@
       <c r="E8" s="1">
         <v>29</v>
       </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="F8" s="1">
+        <v>89</v>
+      </c>
+      <c r="G8" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -604,33 +673,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DC264C-1C4C-4629-A3AD-DD18290371D1}">
-  <dimension ref="C4:H11"/>
+  <dimension ref="C4:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView zoomScale="182" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-    </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-    </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
         <v>3</v>
@@ -639,16 +708,19 @@
         <v>4</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
@@ -661,10 +733,17 @@
       <c r="F9" s="1">
         <v>5</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
         <v>0</v>
       </c>
@@ -677,10 +756,17 @@
       <c r="F10" s="1">
         <v>24</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1">
+        <v>29</v>
+      </c>
+      <c r="I10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
@@ -693,8 +779,15 @@
       <c r="F11" s="1">
         <v>3</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -706,33 +799,36 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058B1D3-8573-4400-BFE1-EA7D88F1B653}">
-  <dimension ref="D6:I27"/>
+  <dimension ref="D6:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>3</v>
@@ -741,82 +837,107 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E11" s="2">
         <v>5.8444634000000004</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>0.79643400000000009</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <v>57.304847000000002</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="4">
+        <v>0.80208699999999999</v>
+      </c>
+      <c r="I11" s="2">
+        <v>5.9472250000000004</v>
+      </c>
+      <c r="J11" s="4">
+        <f>0.000768099*1000</f>
+        <v>0.76809899999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E12" s="2">
         <v>44.089740599999999</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>10.524927</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <v>741.06715399999996</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="4">
+        <v>12.526743</v>
+      </c>
+      <c r="I12" s="2">
+        <v>44.710596000000002</v>
+      </c>
+      <c r="J12" s="4">
+        <v>8.8794570000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="2">
         <v>30.500907599999998</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>6.3886089999999998</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <v>29.386510000000001</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="4">
+        <v>6.3248090000000001</v>
+      </c>
+      <c r="I13" s="2">
+        <v>30.911062000000001</v>
+      </c>
+      <c r="J13" s="4">
+        <v>6.0705989999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
       <c r="E24" s="1" t="s">
         <v>3</v>
@@ -825,62 +946,86 @@
         <v>4</v>
       </c>
       <c r="G24" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I24" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E25" s="2">
         <v>7.1843628000000006</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>0.88687000000000005</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>93.973923999999997</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H25" s="4">
+        <v>2.8815210000000002</v>
+      </c>
+      <c r="I25" s="4">
+        <v>25.193625999999998</v>
+      </c>
+      <c r="J25" s="4">
+        <v>3.3918699999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E26" s="2">
         <v>635.54444599999999</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>215.39219800000001</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>1583.1529559999999</v>
       </c>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H26" s="4">
+        <v>182.01272600000001</v>
+      </c>
+      <c r="I26" s="4">
+        <v>704.452225</v>
+      </c>
+      <c r="J26" s="4">
+        <v>146.106131</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E27" s="2">
         <v>41.875740199999996</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>6.0331799999999998</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="4">
         <v>38.056846</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="H27" s="4">
+        <v>11.740534999999999</v>
+      </c>
+      <c r="I27" s="4">
+        <v>31.007052000000002</v>
+      </c>
+      <c r="J27" s="4">
+        <v>6.8120229999999999</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -894,33 +1039,33 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932C31BC-CD2C-4CF7-B21F-83DAF381D527}">
-  <dimension ref="D6:I30"/>
+  <dimension ref="D6:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView topLeftCell="B6" zoomScale="226" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>3</v>
@@ -929,16 +1074,19 @@
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="I12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
@@ -948,13 +1096,18 @@
       <c r="F13" s="1">
         <v>75</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="2">
         <v>34</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1">
+        <v>74</v>
+      </c>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,15 +1115,20 @@
         <v>32.4</v>
       </c>
       <c r="F14" s="1">
-        <v>3487</v>
-      </c>
-      <c r="G14" s="6">
+        <v>80</v>
+      </c>
+      <c r="G14" s="2">
         <v>29</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>66</v>
+      </c>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
@@ -980,31 +1138,36 @@
       <c r="F15" s="1">
         <v>78</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="2">
         <v>23.75</v>
       </c>
-      <c r="H15" s="1"/>
+      <c r="H15" s="1">
+        <v>72</v>
+      </c>
       <c r="I15" s="1"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
         <v>3</v>
@@ -1013,65 +1176,80 @@
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="8" t="s">
+      <c r="I26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="1">
         <v>32.799999999999997</v>
       </c>
-      <c r="F27" s="9">
-        <v>77</v>
-      </c>
-      <c r="G27" s="7">
+      <c r="F27" s="6">
+        <v>37</v>
+      </c>
+      <c r="G27" s="1">
         <v>29</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="8" t="s">
+      <c r="H27" s="1">
+        <v>31</v>
+      </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D28" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="1">
         <v>31</v>
       </c>
-      <c r="F28" s="9">
-        <v>1728</v>
-      </c>
-      <c r="G28" s="7">
+      <c r="F28" s="6">
+        <v>32</v>
+      </c>
+      <c r="G28" s="1">
         <v>30</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="8" t="s">
+      <c r="H28" s="1">
+        <v>25</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D29" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="1">
         <v>33.4</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="6">
         <v>67</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="1">
         <v>42</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="E30" s="10"/>
+      <c r="H29" s="1">
+        <v>22</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="15">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1084,33 +1262,33 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5232D73-51D5-4B7C-94FC-BB2DBD05F258}">
-  <dimension ref="D6:I29"/>
+  <dimension ref="D6:J29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22:I23"/>
+    <sheetView topLeftCell="C5" zoomScale="234" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
         <v>3</v>
@@ -1119,16 +1297,19 @@
         <v>4</v>
       </c>
       <c r="G12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I12" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1138,13 +1319,18 @@
       <c r="F13" s="1">
         <v>477</v>
       </c>
-      <c r="G13" s="7">
+      <c r="G13" s="1">
         <v>43</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="1">
+        <v>474</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="15">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1152,15 +1338,20 @@
         <v>43</v>
       </c>
       <c r="F14" s="1">
-        <v>8413</v>
-      </c>
-      <c r="G14" s="7">
+        <v>481</v>
+      </c>
+      <c r="G14" s="1">
         <v>41</v>
       </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H14" s="1">
+        <v>475</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="15">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1170,31 +1361,36 @@
       <c r="F15" s="1">
         <v>476</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G15" s="1">
         <v>42</v>
       </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H15" s="1">
+        <v>477</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="15">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
       <c r="E26" s="1" t="s">
         <v>3</v>
@@ -1203,20 +1399,23 @@
         <v>4</v>
       </c>
       <c r="G26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I26" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="1">
         <v>37</v>
       </c>
       <c r="F27" s="1">
@@ -1225,40 +1424,55 @@
       <c r="G27" s="1">
         <v>43</v>
       </c>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H27" s="1">
+        <v>157</v>
+      </c>
+      <c r="I27" s="14"/>
+      <c r="J27" s="15">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D28" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E28" s="7">
+      <c r="E28" s="1">
         <v>36.799999999999997</v>
       </c>
       <c r="F28" s="1">
-        <v>6767</v>
+        <v>318</v>
       </c>
       <c r="G28" s="1">
         <v>1.2</v>
       </c>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H28" s="1">
+        <v>184</v>
+      </c>
+      <c r="I28" s="14"/>
+      <c r="J28" s="15">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="1">
         <v>36.4</v>
       </c>
       <c r="F29" s="1">
-        <v>477</v>
+        <v>417</v>
       </c>
       <c r="G29" s="1">
         <v>43</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="H29" s="1">
+        <v>49</v>
+      </c>
+      <c r="I29" s="14"/>
+      <c r="J29" s="15">
+        <v>234</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1272,33 +1486,36 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AADBA0-93DC-4D36-9539-7EED99A717B7}">
-  <dimension ref="D6:I25"/>
+  <dimension ref="D6:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="B1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>3</v>
@@ -1307,76 +1524,100 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>3.3182526798571428</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="4">
+      <c r="F11" s="4">
+        <v>1.2365999999999999</v>
+      </c>
+      <c r="G11" s="3">
         <v>0.650570339531794</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="7">
+        <v>0.36266666666666664</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="16">
+        <v>0.74053658499999997</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>15.993087296047618</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="4">
+      <c r="F12" s="4">
+        <v>5.1911999999999994</v>
+      </c>
+      <c r="G12" s="3">
         <v>1.036934951990681</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="7">
+        <v>0.12809523809523812</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="16">
+        <v>0.17382682926829268</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>1.3335248047619047E-2</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="4">
+      <c r="F13" s="4">
+        <v>4.564E-2</v>
+      </c>
+      <c r="G13" s="3">
         <v>1.1419826562737265E-3</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D18" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="7">
+        <v>1.8448571428571431E-4</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="16">
+        <v>1.3268292682926829E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
         <v>3</v>
@@ -1385,56 +1626,80 @@
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>21.272810870952384</v>
       </c>
-      <c r="F23" s="1"/>
-      <c r="G23" s="5">
+      <c r="F23" s="10">
+        <v>11.608181800000001</v>
+      </c>
+      <c r="G23" s="4">
         <v>22.009695432753144</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="8">
+        <v>5.1454545454545455</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="10">
+        <v>19.90041463</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>54.366213445238088</v>
       </c>
-      <c r="F24" s="1"/>
-      <c r="G24" s="5">
+      <c r="F24" s="4">
+        <v>27.88181818</v>
+      </c>
+      <c r="G24" s="4">
         <v>41.962133167440179</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="4">
+        <v>9.877272727272727</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="10">
+        <v>32.018295119999998</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>0.20266894885714284</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" s="5">
+      <c r="F25" s="10">
+        <v>0.13765454999999999</v>
+      </c>
+      <c r="G25" s="4">
         <v>0.31562325209414455</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="H25" s="4">
+        <v>6.4690909000000005E-2</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="10">
+        <v>0.24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1447,36 +1712,36 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F2AC6CE-64BB-4478-B736-E99BE9C1E616}">
-  <dimension ref="D6:I25"/>
+  <dimension ref="D6:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="254" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+    </row>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
       <c r="E10" s="1" t="s">
         <v>3</v>
@@ -1485,76 +1750,100 @@
         <v>4</v>
       </c>
       <c r="G10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>441.17578129999998</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="9">
+        <v>541.37255900000002</v>
+      </c>
       <c r="G11" s="2">
         <v>424.90498991935482</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H11" s="2">
+        <v>1142.6389509999999</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="19">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="2">
         <v>296.69903269999998</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="2">
+        <v>268.01928709999999</v>
+      </c>
       <c r="G12" s="2">
         <v>362.37865423387098</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H12" s="2">
+        <v>866.27027529999998</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="19">
+        <v>247.2222222</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="2">
         <v>45.33984375</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="2">
+        <v>47.77734375</v>
+      </c>
       <c r="G13" s="2">
         <v>435.81161794354841</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-    </row>
-    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D18" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="2">
+        <v>462.0563616</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="19">
+        <v>9.9631111109999999</v>
+      </c>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
       <c r="E22" s="1" t="s">
         <v>3</v>
@@ -1563,56 +1852,80 @@
         <v>4</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="I22" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D23" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E23" s="2">
         <v>456.52734379999998</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="2">
+        <v>669.93572400000005</v>
+      </c>
       <c r="G23" s="2">
         <v>458.7109375</v>
       </c>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H23" s="2">
+        <v>1193.5823863636363</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="17">
+        <v>374.6341463</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" ht="16" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="2">
         <v>919.13244050000003</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="2">
+        <v>937.67578130000004</v>
+      </c>
       <c r="G24" s="2">
         <v>616.30255681818187</v>
       </c>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="H24" s="2">
+        <v>1034.9904119318182</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="18">
+        <v>586.34146299999998</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="2">
         <v>49.633370540000001</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="2">
+        <v>52.381392050000002</v>
+      </c>
       <c r="G25" s="2">
         <v>437.71164772727275</v>
       </c>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
+      <c r="H25" s="2">
+        <v>465.88245738636363</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="17">
+        <v>30</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
add last benchmark results
</commit_message>
<xml_diff>
--- a/results/Global performance comparison.xlsx
+++ b/results/Global performance comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yohan/containers-comparison/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{433638A2-4688-C04E-A229-EEFF6895732B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C53265-A384-EB47-AF34-0C7E5638ECBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10540" yWindow="-28800" windowWidth="51200" windowHeight="28800" activeTab="6" xr2:uid="{2794598E-EB7C-45E9-952E-510353A79499}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="6" xr2:uid="{2794598E-EB7C-45E9-952E-510353A79499}"/>
   </bookViews>
   <sheets>
     <sheet name="build" sheetId="1" r:id="rId1"/>
@@ -243,9 +243,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -254,6 +251,9 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +571,7 @@
   <dimension ref="C5:H14"/>
   <sheetViews>
     <sheetView zoomScale="206" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5:G8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -643,22 +643,22 @@
       </c>
     </row>
     <row r="13" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19"/>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="19"/>
+      <c r="G14" s="19"/>
+      <c r="H14" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -682,22 +682,22 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="4" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
     </row>
     <row r="5" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C8" s="1"/>
@@ -801,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B058B1D3-8573-4400-BFE1-EA7D88F1B653}">
   <dimension ref="D6:J27"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
@@ -811,22 +811,22 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
@@ -920,22 +920,22 @@
       </c>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="20" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
     </row>
     <row r="24" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
@@ -1041,29 +1041,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{932C31BC-CD2C-4CF7-B21F-83DAF381D527}">
   <dimension ref="D6:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="226" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView topLeftCell="B9" zoomScale="170" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
@@ -1102,7 +1102,9 @@
       <c r="H13" s="1">
         <v>74</v>
       </c>
-      <c r="I13" s="1"/>
+      <c r="I13" s="1">
+        <v>27</v>
+      </c>
       <c r="J13" s="1">
         <v>58</v>
       </c>
@@ -1123,7 +1125,9 @@
       <c r="H14" s="1">
         <v>66</v>
       </c>
-      <c r="I14" s="1"/>
+      <c r="I14" s="1">
+        <v>28</v>
+      </c>
       <c r="J14" s="1">
         <v>64</v>
       </c>
@@ -1144,28 +1148,30 @@
       <c r="H15" s="1">
         <v>72</v>
       </c>
-      <c r="I15" s="1"/>
+      <c r="I15" s="1">
+        <v>35</v>
+      </c>
       <c r="J15" s="1">
         <v>70</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
@@ -1181,10 +1187,10 @@
       <c r="H26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="I26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1204,8 +1210,10 @@
       <c r="H27" s="1">
         <v>31</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15">
+      <c r="I27" s="13">
+        <v>22</v>
+      </c>
+      <c r="J27" s="14">
         <v>31</v>
       </c>
     </row>
@@ -1225,8 +1233,10 @@
       <c r="H28" s="1">
         <v>25</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15">
+      <c r="I28" s="13">
+        <v>21</v>
+      </c>
+      <c r="J28" s="14">
         <v>21</v>
       </c>
     </row>
@@ -1246,8 +1256,10 @@
       <c r="H29" s="1">
         <v>22</v>
       </c>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15">
+      <c r="I29" s="13">
+        <v>22</v>
+      </c>
+      <c r="J29" s="14">
         <v>15</v>
       </c>
     </row>
@@ -1264,29 +1276,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5232D73-51D5-4B7C-94FC-BB2DBD05F258}">
   <dimension ref="D6:J29"/>
   <sheetViews>
-    <sheetView topLeftCell="C5" zoomScale="234" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView topLeftCell="C11" zoomScale="234" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="12" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D12" s="1"/>
@@ -1302,10 +1314,10 @@
       <c r="H12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="13" t="s">
+      <c r="J12" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1325,8 +1337,10 @@
       <c r="H13" s="1">
         <v>474</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="15">
+      <c r="I13" s="13">
+        <v>43</v>
+      </c>
+      <c r="J13" s="14">
         <v>472</v>
       </c>
     </row>
@@ -1346,8 +1360,10 @@
       <c r="H14" s="1">
         <v>475</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="15">
+      <c r="I14" s="13">
+        <v>43</v>
+      </c>
+      <c r="J14" s="14">
         <v>481</v>
       </c>
     </row>
@@ -1367,28 +1383,30 @@
       <c r="H15" s="1">
         <v>477</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="15">
+      <c r="I15" s="13">
+        <v>43</v>
+      </c>
+      <c r="J15" s="14">
         <v>476</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="26" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D26" s="1"/>
@@ -1404,10 +1422,10 @@
       <c r="H26" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="I26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1427,8 +1445,10 @@
       <c r="H27" s="1">
         <v>157</v>
       </c>
-      <c r="I27" s="14"/>
-      <c r="J27" s="15">
+      <c r="I27" s="1">
+        <v>37</v>
+      </c>
+      <c r="J27" s="14">
         <v>68</v>
       </c>
     </row>
@@ -1448,8 +1468,10 @@
       <c r="H28" s="1">
         <v>184</v>
       </c>
-      <c r="I28" s="14"/>
-      <c r="J28" s="15">
+      <c r="I28" s="1">
+        <v>35</v>
+      </c>
+      <c r="J28" s="14">
         <v>74</v>
       </c>
     </row>
@@ -1469,8 +1491,10 @@
       <c r="H29" s="1">
         <v>49</v>
       </c>
-      <c r="I29" s="14"/>
-      <c r="J29" s="15">
+      <c r="I29" s="1">
+        <v>36</v>
+      </c>
+      <c r="J29" s="14">
         <v>234</v>
       </c>
     </row>
@@ -1489,7 +1513,7 @@
   <dimension ref="D6:J25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1498,22 +1522,22 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
@@ -1529,10 +1553,10 @@
       <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1552,8 +1576,10 @@
       <c r="H11" s="7">
         <v>0.36266666666666664</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="16">
+      <c r="I11" s="13">
+        <v>1.32</v>
+      </c>
+      <c r="J11" s="15">
         <v>0.74053658499999997</v>
       </c>
     </row>
@@ -1573,8 +1599,10 @@
       <c r="H12" s="7">
         <v>0.12809523809523812</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="16">
+      <c r="I12" s="13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J12" s="15">
         <v>0.17382682926829268</v>
       </c>
     </row>
@@ -1594,28 +1622,30 @@
       <c r="H13" s="7">
         <v>1.8448571428571431E-4</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="16">
+      <c r="I13" s="13">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J13" s="15">
         <v>1.3268292682926829E-2</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
@@ -1631,10 +1661,10 @@
       <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1654,7 +1684,9 @@
       <c r="H23" s="8">
         <v>5.1454545454545455</v>
       </c>
-      <c r="I23" s="14"/>
+      <c r="I23" s="13">
+        <v>50</v>
+      </c>
       <c r="J23" s="10">
         <v>19.90041463</v>
       </c>
@@ -1675,7 +1707,9 @@
       <c r="H24" s="4">
         <v>9.877272727272727</v>
       </c>
-      <c r="I24" s="14"/>
+      <c r="I24" s="13">
+        <v>60</v>
+      </c>
       <c r="J24" s="10">
         <v>32.018295119999998</v>
       </c>
@@ -1685,20 +1719,22 @@
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <v>0.20266894885714284</v>
+        <v>2</v>
       </c>
       <c r="F25" s="10">
-        <v>0.13765454999999999</v>
+        <v>1.4</v>
       </c>
       <c r="G25" s="4">
-        <v>0.31562325209414455</v>
+        <v>3</v>
       </c>
       <c r="H25" s="4">
-        <v>6.4690909000000005E-2</v>
-      </c>
-      <c r="I25" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="I25" s="13">
+        <v>12</v>
+      </c>
       <c r="J25" s="10">
-        <v>0.24</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1715,7 +1751,7 @@
   <dimension ref="D6:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C5" zoomScale="254" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1724,22 +1760,22 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
     </row>
     <row r="7" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
     </row>
     <row r="10" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D10" s="1"/>
@@ -1755,10 +1791,10 @@
       <c r="H10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="I10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J10" s="13" t="s">
+      <c r="J10" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1778,8 +1814,10 @@
       <c r="H11" s="2">
         <v>1142.6389509999999</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="19">
+      <c r="I11" s="2">
+        <v>379</v>
+      </c>
+      <c r="J11" s="18">
         <v>350</v>
       </c>
     </row>
@@ -1799,8 +1837,10 @@
       <c r="H12" s="2">
         <v>866.27027529999998</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="19">
+      <c r="I12" s="2">
+        <v>322</v>
+      </c>
+      <c r="J12" s="18">
         <v>247.2222222</v>
       </c>
     </row>
@@ -1820,28 +1860,30 @@
       <c r="H13" s="2">
         <v>462.0563616</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="19">
+      <c r="I13" s="2">
+        <v>12</v>
+      </c>
+      <c r="J13" s="18">
         <v>9.9631111109999999</v>
       </c>
     </row>
     <row r="18" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
     </row>
     <row r="19" spans="4:10" x14ac:dyDescent="0.2">
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.2">
       <c r="D22" s="1"/>
@@ -1857,10 +1899,10 @@
       <c r="H22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1880,8 +1922,8 @@
       <c r="H23" s="2">
         <v>1193.5823863636363</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="17">
+      <c r="I23" s="13"/>
+      <c r="J23" s="16">
         <v>374.6341463</v>
       </c>
     </row>
@@ -1901,8 +1943,8 @@
       <c r="H24" s="2">
         <v>1034.9904119318182</v>
       </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="18">
+      <c r="I24" s="13"/>
+      <c r="J24" s="17">
         <v>586.34146299999998</v>
       </c>
     </row>
@@ -1922,8 +1964,8 @@
       <c r="H25" s="2">
         <v>465.88245738636363</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="17">
+      <c r="I25" s="13"/>
+      <c r="J25" s="16">
         <v>30</v>
       </c>
     </row>

</xml_diff>